<commit_message>
Se limpia la clase del stepDefinitions se envia código al directorio questions.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DatosPruebaDatepicker.xlsx
+++ b/src/test/resources/data/DatosPruebaDatepicker.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29607"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEDB0ABE-BB3F-4A79-A3C7-736BD4FF1B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FB6C6D1-5182-4DB1-8839-7F4ADC0181E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,16 +33,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>caso</t>
+    <t>case</t>
   </si>
   <si>
-    <t>fecha</t>
+    <t>date</t>
   </si>
   <si>
     <t>fecha_mes_diferente</t>
   </si>
   <si>
-    <t>02/15/2025</t>
+    <t>02/15/2026</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>